<commit_message>
Model training and Evaluation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="preprocessing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="confusionmatrix" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,75 +435,147 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ham</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>go jurong point, crazy.. available bugis n great world la e buffet... cine got amore wat...</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ham</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ok lar... joking wif u oni...</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>spam</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>free entry 2 wkly comp win fa cup final tkts 21st may 2005. text fa 87121 receive entry question(std txt rate)t&amp;c's apply 08452810075over18's</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ham</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>u dun say early hor... u c already say...</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ham</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nah think go usf, life around though</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>ham</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>spam</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>ham</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>go jurong point, crazy.. available bugis n great world la e buffet... cine got amore wat...</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ham</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ok lar... joking wif u oni...</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>spam</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>free entry 2 wkly comp win fa cup final tkts 21st may 2005. text fa 87121 receive entry question(std txt rate)t&amp;c's apply 08452810075over18's</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ham</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>u dun say early hor... u c already say...</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ham</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>nah think go usf, life around though</t>
-        </is>
+      <c r="B3" t="n">
+        <v>34</v>
+      </c>
+      <c r="C3" t="n">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>